<commit_message>
Docs - Fix - Refactor: Ajustando análises e modelos do supervisionado para posíveis usuários. Alterando label da planilha de possíveis usuários
</commit_message>
<xml_diff>
--- a/dados_possiveis_usuarios_c_label.xlsx
+++ b/dados_possiveis_usuarios_c_label.xlsx
@@ -550,7 +550,7 @@
       </c>
       <c r="W1" s="1" t="inlineStr">
         <is>
-          <t>Usaria o aplicativo</t>
+          <t>Usaria o aplicativo?</t>
         </is>
       </c>
     </row>
@@ -653,7 +653,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -2651,7 +2651,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W26" t="inlineStr"/>
+      <c r="W26" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
@@ -3024,7 +3028,7 @@
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -3127,7 +3131,7 @@
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -3230,7 +3234,7 @@
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -3726,7 +3730,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W39" t="inlineStr"/>
+      <c r="W39" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="40">
       <c r="A40" t="n">
@@ -4260,7 +4268,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W45" t="inlineStr"/>
+      <c r="W45" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
@@ -4361,7 +4373,7 @@
       </c>
       <c r="W46" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -4675,7 +4687,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W50" t="inlineStr"/>
+      <c r="W50" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
@@ -4894,7 +4910,7 @@
       </c>
       <c r="W53" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -5242,7 +5258,7 @@
       </c>
       <c r="W57" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -5584,7 +5600,11 @@
           <t>Não</t>
         </is>
       </c>
-      <c r="W61" t="inlineStr"/>
+      <c r="W61" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
@@ -5833,7 +5853,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W64" t="inlineStr"/>
+      <c r="W64" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
@@ -6177,7 +6201,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W68" t="inlineStr"/>
+      <c r="W68" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
@@ -6371,7 +6399,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W70" t="inlineStr"/>
+      <c r="W70" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
@@ -6899,7 +6931,7 @@
       </c>
       <c r="W76" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -7186,7 +7218,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W79" t="inlineStr"/>
+      <c r="W79" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
@@ -7403,7 +7439,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W82" t="inlineStr"/>
+      <c r="W82" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
@@ -7679,7 +7719,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W86" t="inlineStr"/>
+      <c r="W86" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
@@ -8306,7 +8350,7 @@
       </c>
       <c r="W93" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -8409,7 +8453,7 @@
       </c>
       <c r="W94" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -8846,7 +8890,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W99" t="inlineStr"/>
+      <c r="W99" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
@@ -8947,7 +8995,7 @@
       </c>
       <c r="W100" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -9143,7 +9191,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W102" t="inlineStr"/>
+      <c r="W102" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
@@ -9671,7 +9723,7 @@
       </c>
       <c r="W108" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -9869,7 +9921,7 @@
       </c>
       <c r="W110" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -10278,7 +10330,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W115" t="inlineStr"/>
+      <c r="W115" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
@@ -10377,7 +10433,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W116" t="inlineStr"/>
+      <c r="W116" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
@@ -10537,7 +10597,7 @@
       </c>
       <c r="W118" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -10948,7 +11008,7 @@
       </c>
       <c r="W123" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -11450,7 +11510,7 @@
       </c>
       <c r="W129" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -11889,7 +11949,7 @@
       </c>
       <c r="W134" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -12081,7 +12141,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W136" t="inlineStr"/>
+      <c r="W136" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
@@ -12482,7 +12546,7 @@
       </c>
       <c r="W141" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -12583,7 +12647,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W142" t="inlineStr"/>
+      <c r="W142" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="143">
       <c r="A143" t="n">
@@ -12682,7 +12750,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W143" t="inlineStr"/>
+      <c r="W143" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="144">
       <c r="A144" t="n">
@@ -12783,7 +12855,7 @@
       </c>
       <c r="W144" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -13304,7 +13376,7 @@
       </c>
       <c r="W151" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -13407,7 +13479,7 @@
       </c>
       <c r="W152" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -13508,7 +13580,11 @@
           <t>Não</t>
         </is>
       </c>
-      <c r="W153" t="inlineStr"/>
+      <c r="W153" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="154">
       <c r="A154" t="n">
@@ -13666,7 +13742,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W155" t="inlineStr"/>
+      <c r="W155" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="156">
       <c r="A156" t="n">
@@ -13765,7 +13845,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W156" t="inlineStr"/>
+      <c r="W156" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="157">
       <c r="A157" t="n">
@@ -13923,7 +14007,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W158" t="inlineStr"/>
+      <c r="W158" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="159">
       <c r="A159" t="n">
@@ -14024,7 +14112,7 @@
       </c>
       <c r="W159" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -14393,7 +14481,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W164" t="inlineStr"/>
+      <c r="W164" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="165">
       <c r="A165" t="n">
@@ -14551,7 +14643,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W166" t="inlineStr"/>
+      <c r="W166" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="167">
       <c r="A167" t="n">
@@ -14743,7 +14839,7 @@
       </c>
       <c r="W168" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -14905,7 +15001,7 @@
       </c>
       <c r="W170" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -15006,7 +15102,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W171" t="inlineStr"/>
+      <c r="W171" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="172">
       <c r="A172" t="n">
@@ -15198,7 +15298,7 @@
       </c>
       <c r="W173" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -15730,7 +15830,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W179" t="inlineStr"/>
+      <c r="W179" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="180">
       <c r="A180" t="n">
@@ -15829,7 +15933,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W180" t="inlineStr"/>
+      <c r="W180" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="181">
       <c r="A181" t="n">
@@ -16023,7 +16131,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W182" t="inlineStr"/>
+      <c r="W182" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
@@ -16122,7 +16234,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W183" t="inlineStr"/>
+      <c r="W183" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
@@ -16221,7 +16337,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W184" t="inlineStr"/>
+      <c r="W184" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
@@ -16320,7 +16440,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W185" t="inlineStr"/>
+      <c r="W185" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
@@ -16421,7 +16545,7 @@
       </c>
       <c r="W186" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -16678,7 +16802,7 @@
       </c>
       <c r="W189" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -16779,7 +16903,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W190" t="inlineStr"/>
+      <c r="W190" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="191">
       <c r="A191" t="n">
@@ -17237,7 +17365,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W196" t="inlineStr"/>
+      <c r="W196" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="197">
       <c r="A197" t="n">
@@ -17336,7 +17468,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W197" t="inlineStr"/>
+      <c r="W197" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="198">
       <c r="A198" t="n">
@@ -17437,7 +17573,7 @@
       </c>
       <c r="W198" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -17692,7 +17828,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W201" t="inlineStr"/>
+      <c r="W201" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
@@ -18028,7 +18168,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W205" t="inlineStr"/>
+      <c r="W205" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
@@ -18127,7 +18271,11 @@
           <t>Não</t>
         </is>
       </c>
-      <c r="W206" t="inlineStr"/>
+      <c r="W206" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
@@ -18226,7 +18374,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W207" t="inlineStr"/>
+      <c r="W207" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
@@ -18513,7 +18665,7 @@
       </c>
       <c r="W210" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -18614,7 +18766,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W211" t="inlineStr"/>
+      <c r="W211" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
@@ -18772,7 +18928,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W213" t="inlineStr"/>
+      <c r="W213" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
@@ -19209,7 +19369,7 @@
       </c>
       <c r="W218" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -19555,7 +19715,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W222" t="inlineStr"/>
+      <c r="W222" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
@@ -19899,7 +20063,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W226" t="inlineStr"/>
+      <c r="W226" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
@@ -20176,7 +20344,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W229" t="inlineStr"/>
+      <c r="W229" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="230">
       <c r="A230" t="n">
@@ -20275,7 +20447,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W230" t="inlineStr"/>
+      <c r="W230" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="231">
       <c r="A231" t="n">
@@ -20435,7 +20611,7 @@
       </c>
       <c r="W232" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -20633,7 +20809,7 @@
       </c>
       <c r="W234" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -20827,7 +21003,7 @@
       </c>
       <c r="W236" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -20930,7 +21106,7 @@
       </c>
       <c r="W237" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -21031,7 +21207,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W238" t="inlineStr"/>
+      <c r="W238" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
@@ -21130,7 +21310,11 @@
           <t>Sim</t>
         </is>
       </c>
-      <c r="W239" t="inlineStr"/>
+      <c r="W239" t="inlineStr">
+        <is>
+          <t>Sim</t>
+        </is>
+      </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
@@ -21322,7 +21506,7 @@
       </c>
       <c r="W241" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -21543,7 +21727,7 @@
       </c>
       <c r="W244" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>
@@ -21828,7 +22012,7 @@
       </c>
       <c r="W247" t="inlineStr">
         <is>
-          <t>Sim</t>
+          <t>Não</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Feat - Refactor - Test: Criando forms para implementação do modelo de possíveis assinantes e testando modelo com dados criados
</commit_message>
<xml_diff>
--- a/dados_possiveis_usuarios_c_label.xlsx
+++ b/dados_possiveis_usuarios_c_label.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -653,7 +653,7 @@
       </c>
       <c r="W2" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -1590,7 +1590,7 @@
       </c>
       <c r="W13" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -1883,7 +1883,7 @@
       </c>
       <c r="W16" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -2282,7 +2282,7 @@
       </c>
       <c r="W21" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -3028,7 +3028,7 @@
       </c>
       <c r="W31" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -3131,7 +3131,7 @@
       </c>
       <c r="W32" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -3234,7 +3234,7 @@
       </c>
       <c r="W33" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -4373,7 +4373,7 @@
       </c>
       <c r="W46" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -4910,7 +4910,7 @@
       </c>
       <c r="W53" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -5258,7 +5258,7 @@
       </c>
       <c r="W57" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -6931,7 +6931,7 @@
       </c>
       <c r="W76" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -8350,7 +8350,7 @@
       </c>
       <c r="W93" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -8453,7 +8453,7 @@
       </c>
       <c r="W94" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -8995,7 +8995,7 @@
       </c>
       <c r="W100" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -9723,7 +9723,7 @@
       </c>
       <c r="W108" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -9921,7 +9921,7 @@
       </c>
       <c r="W110" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -10597,7 +10597,7 @@
       </c>
       <c r="W118" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -11008,7 +11008,7 @@
       </c>
       <c r="W123" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -11510,7 +11510,7 @@
       </c>
       <c r="W129" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -11949,7 +11949,7 @@
       </c>
       <c r="W134" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -12546,7 +12546,7 @@
       </c>
       <c r="W141" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -12855,7 +12855,7 @@
       </c>
       <c r="W144" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -13376,7 +13376,7 @@
       </c>
       <c r="W151" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -13479,7 +13479,7 @@
       </c>
       <c r="W152" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -14112,7 +14112,7 @@
       </c>
       <c r="W159" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -14839,7 +14839,7 @@
       </c>
       <c r="W168" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -15001,7 +15001,7 @@
       </c>
       <c r="W170" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -15298,7 +15298,7 @@
       </c>
       <c r="W173" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -16545,7 +16545,7 @@
       </c>
       <c r="W186" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -16802,7 +16802,7 @@
       </c>
       <c r="W189" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -17573,7 +17573,7 @@
       </c>
       <c r="W198" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -18665,7 +18665,7 @@
       </c>
       <c r="W210" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -19369,7 +19369,7 @@
       </c>
       <c r="W218" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -20611,7 +20611,7 @@
       </c>
       <c r="W232" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -20809,7 +20809,7 @@
       </c>
       <c r="W234" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -21003,7 +21003,7 @@
       </c>
       <c r="W236" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -21106,7 +21106,7 @@
       </c>
       <c r="W237" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -21506,7 +21506,7 @@
       </c>
       <c r="W241" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -21727,7 +21727,7 @@
       </c>
       <c r="W244" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>
@@ -22012,7 +22012,7 @@
       </c>
       <c r="W247" t="inlineStr">
         <is>
-          <t>Não</t>
+          <t>Sim</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Docs - Arrumando documentação e finalizando arquivos de para a predição de  possíveis usuários.
</commit_message>
<xml_diff>
--- a/dados_possiveis_usuarios_c_label.xlsx
+++ b/dados_possiveis_usuarios_c_label.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>